<commit_message>
fix(data-capture): set id attribute type to INT
</commit_message>
<xml_diff>
--- a/data-capture/emx2/emx2-cde-fdp-rml-compat-v2.xlsx
+++ b/data-capture/emx2/emx2-cde-fdp-rml-compat-v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/cde-in-box/data-capture/emx2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FC923D-7FA9-0049-A6A9-F611264C6F16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE72C889-E3B9-2940-8408-089581BAB719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29420" yWindow="-9200" windowWidth="27380" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38860" yWindow="-13220" windowWidth="27380" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="360">
   <si>
     <t>tableName</t>
   </si>
@@ -1101,6 +1101,9 @@
   </si>
   <si>
     <t>2020-09-22T22:22:00</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -1480,14 +1483,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="3" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
@@ -1545,7 +1549,9 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>359</v>
+      </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2529,25 +2535,25 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">RANDBETWEEN(DATE(1930,1,1),DATE(2010,12,31))</f>
-        <v>21195</v>
+        <v>35949</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>39518</v>
+        <v>23123</v>
       </c>
       <c r="I2" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>38413</v>
+        <v>27961</v>
       </c>
       <c r="J2" t="s">
         <v>52</v>
       </c>
       <c r="K2" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>34392</v>
+        <v>31835</v>
       </c>
       <c r="L2" t="s">
         <v>64</v>
@@ -2557,7 +2563,7 @@
       </c>
       <c r="N2" s="1">
         <f ca="1">RANDBETWEEN(DATE(2000,1,1),DATE(2050,12,31))</f>
-        <v>49605</v>
+        <v>51759</v>
       </c>
       <c r="O2" t="s">
         <v>76</v>
@@ -2641,25 +2647,25 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F11" ca="1" si="0">RANDBETWEEN(DATE(1930,1,1),DATE(2010,12,31))</f>
-        <v>33647</v>
+        <v>26420</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>27168</v>
+        <v>31687</v>
       </c>
       <c r="I3" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>35788</v>
+        <v>39407</v>
       </c>
       <c r="J3" t="s">
         <v>53</v>
       </c>
       <c r="K3" s="1">
         <f ca="1">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>34528</v>
+        <v>32807</v>
       </c>
       <c r="L3" t="s">
         <v>65</v>
@@ -2669,7 +2675,7 @@
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N11" ca="1" si="1">RANDBETWEEN(DATE(2000,1,1),DATE(2050,12,31))</f>
-        <v>43948</v>
+        <v>42980</v>
       </c>
       <c r="O3" t="s">
         <v>76</v>
@@ -2753,25 +2759,25 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12329</v>
+        <v>36750</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ref="H4:K11" ca="1" si="2">RANDBETWEEN(DATE(1960,1,1),DATE(2010,12,31))</f>
-        <v>36848</v>
+        <v>24779</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>35533</v>
+        <v>36798</v>
       </c>
       <c r="J4" t="s">
         <v>54</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>35295</v>
+        <v>36410</v>
       </c>
       <c r="L4" t="s">
         <v>66</v>
@@ -2781,7 +2787,7 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>47389</v>
+        <v>41926</v>
       </c>
       <c r="O4" t="s">
         <v>77</v>
@@ -2865,25 +2871,25 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14993</v>
+        <v>38052</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28922</v>
+        <v>27320</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>36428</v>
+        <v>27149</v>
       </c>
       <c r="J5" t="s">
         <v>55</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>39320</v>
+        <v>25782</v>
       </c>
       <c r="L5" t="s">
         <v>67</v>
@@ -2893,7 +2899,7 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>41041</v>
+        <v>41153</v>
       </c>
       <c r="O5" t="s">
         <v>77</v>
@@ -2977,25 +2983,25 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>38087</v>
+        <v>21306</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28938</v>
+        <v>38974</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>38891</v>
+        <v>25261</v>
       </c>
       <c r="J6" t="s">
         <v>56</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>37180</v>
+        <v>34901</v>
       </c>
       <c r="L6" t="s">
         <v>68</v>
@@ -3005,7 +3011,7 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>53738</v>
+        <v>37792</v>
       </c>
       <c r="O6" t="s">
         <v>77</v>
@@ -3089,25 +3095,25 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>38073</v>
+        <v>27568</v>
       </c>
       <c r="G7" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>32875</v>
+        <v>26766</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40218</v>
+        <v>29164</v>
       </c>
       <c r="J7" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23878</v>
+        <v>33405</v>
       </c>
       <c r="L7" t="s">
         <v>69</v>
@@ -3117,7 +3123,7 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45109</v>
+        <v>54975</v>
       </c>
       <c r="O7" t="s">
         <v>76</v>
@@ -3201,25 +3207,25 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18722</v>
+        <v>18044</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>31899</v>
+        <v>29247</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23736</v>
+        <v>27875</v>
       </c>
       <c r="J8" t="s">
         <v>58</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>39147</v>
+        <v>27547</v>
       </c>
       <c r="L8" t="s">
         <v>70</v>
@@ -3229,7 +3235,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>48858</v>
+        <v>41648</v>
       </c>
       <c r="O8" t="s">
         <v>76</v>
@@ -3313,25 +3319,25 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>39128</v>
+        <v>40428</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27214</v>
+        <v>39168</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23008</v>
+        <v>35070</v>
       </c>
       <c r="J9" t="s">
         <v>59</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28649</v>
+        <v>30422</v>
       </c>
       <c r="L9" t="s">
         <v>71</v>
@@ -3341,7 +3347,7 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>54259</v>
+        <v>54036</v>
       </c>
       <c r="O9" t="s">
         <v>77</v>
@@ -3425,25 +3431,25 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24247</v>
+        <v>38012</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>24145</v>
+        <v>22547</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>32651</v>
+        <v>35760</v>
       </c>
       <c r="J10" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28562</v>
+        <v>39799</v>
       </c>
       <c r="L10" t="s">
         <v>72</v>
@@ -3453,7 +3459,7 @@
       </c>
       <c r="N10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>39453</v>
+        <v>49794</v>
       </c>
       <c r="O10" t="s">
         <v>77</v>
@@ -3537,25 +3543,25 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24056</v>
+        <v>14422</v>
       </c>
       <c r="G11" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28165</v>
+        <v>23138</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>35853</v>
+        <v>25424</v>
       </c>
       <c r="J11" t="s">
         <v>61</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27711</v>
+        <v>25941</v>
       </c>
       <c r="L11" t="s">
         <v>73</v>
@@ -3565,7 +3571,7 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43840</v>
+        <v>45713</v>
       </c>
       <c r="O11" t="s">
         <v>77</v>

</xml_diff>